<commit_message>
fix bai toán tăng giá và thêm readme cho các thư mục
</commit_message>
<xml_diff>
--- a/4_MOBILE_DEV/ch04_Pandas/output-data.xlsx
+++ b/4_MOBILE_DEV/ch04_Pandas/output-data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,172 +456,166 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr"/>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Age</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>City</t>
+        </is>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>stt</t>
-        </is>
+      <c r="A3" t="n">
+        <v>1</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Age</t>
-        </is>
+          <t>John</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>27</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>City</t>
+          <t>Newyork</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>John</t>
+          <t>Nancy</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Newyork</t>
+          <t>Paris</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Nancy</t>
+          <t>Bob</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Paris</t>
+          <t>London</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Bob</t>
+          <t>Job</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>London</t>
+          <t>Ha Noi</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Job</t>
+          <t>Coney</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Ha Noi</t>
+          <t>Bejing</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Coney</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Bejing</t>
+          <t>Hongkong</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Smith</t>
+          <t>Kenvin</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Hongkong</t>
+          <t>HCM</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Kenvin</t>
+          <t>Vic</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>21</v>
+        <v>90</v>
       </c>
       <c r="D10" t="inlineStr">
-        <is>
-          <t>HCM</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>8</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Vic</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>90</v>
-      </c>
-      <c r="D11" t="inlineStr">
         <is>
           <t>San Joe</t>
         </is>

</xml_diff>